<commit_message>
Did 3 new skill documentation for hunter.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Fighter/Documentation/FighterSkills.xlsx
+++ b/GameDesign/Class/Fighter/Documentation/FighterSkills.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1-FighterMeditation" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="9-KiBlast" sheetId="11" r:id="rId9"/>
     <sheet name="10-LiquidKick" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -150,9 +150,6 @@
     <t>[[Boost the next ''Iron Punch'' by 20%]] (1 turn)</t>
   </si>
   <si>
-    <t>Move opposite dirrection from target.</t>
-  </si>
-  <si>
     <t>[[Range: 1 ]]</t>
   </si>
   <si>
@@ -298,6 +295,9 @@
   </si>
   <si>
     <t>If is an enemy, [[Damage:  27-30 earth ]]</t>
+  </si>
+  <si>
+    <t>Move opposite direction from target.</t>
   </si>
 </sst>
 </file>
@@ -872,14 +872,14 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -923,7 +923,7 @@
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -963,7 +963,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -975,14 +975,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -994,14 +994,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1037,7 +1037,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1049,7 +1049,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1061,28 +1061,28 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1112,7 +1112,7 @@
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
       <c r="C28" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -1245,14 +1245,14 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1282,7 +1282,7 @@
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1296,7 +1296,7 @@
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -1436,7 +1436,7 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1480,7 +1480,7 @@
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -1499,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,7 +1532,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1551,7 +1551,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1611,21 +1611,21 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1655,7 +1655,7 @@
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -1807,7 +1807,7 @@
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,7 +1891,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1903,7 +1903,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1922,7 +1922,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1996,7 +1996,7 @@
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="6" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2040,7 +2040,7 @@
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
       <c r="C28" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -2080,7 +2080,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2092,7 +2092,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2111,7 +2111,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2130,14 +2130,14 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2156,7 +2156,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2180,7 +2180,7 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2210,7 +2210,7 @@
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2250,7 +2250,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2262,7 +2262,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2274,14 +2274,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2348,14 +2348,14 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2385,7 +2385,7 @@
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -2425,7 +2425,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2437,14 +2437,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -2456,14 +2456,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2475,7 +2475,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -2501,7 +2501,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2525,21 +2525,21 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1"/>
     </row>

</xml_diff>

<commit_message>
Documentation of the Guardian skills done.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Fighter/Documentation/FighterSkills.xlsx
+++ b/GameDesign/Class/Fighter/Documentation/FighterSkills.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1-FighterMeditation" sheetId="2" r:id="rId1"/>
@@ -1499,7 +1499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1674,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>